<commit_message>
Capstone  week 6 chnages saturday
</commit_message>
<xml_diff>
--- a/CapsStone/Project-Report/Project-Report-addons.xlsx
+++ b/CapsStone/Project-Report/Project-Report-addons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aamol\Repos\GithubRepos\msdatascience\msdatascience\CapsStone\Project Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF259A3F-9001-4C52-8E77-26B993E08AE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F28CA49-4529-4B4D-8521-870FD928DC37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="203">
   <si>
     <t>Logisitic Regression</t>
   </si>
@@ -311,9 +311,6 @@
     <t>Return on equity ratio</t>
   </si>
   <si>
-    <t>Wprking capital ratio</t>
-  </si>
-  <si>
     <t>Variable</t>
   </si>
   <si>
@@ -621,6 +618,39 @@
   </si>
   <si>
     <t>Glmnet (Ridge regression)</t>
+  </si>
+  <si>
+    <t>restm_nopi_mag</t>
+  </si>
+  <si>
+    <t>sstk</t>
+  </si>
+  <si>
+    <t>de_ratio</t>
+  </si>
+  <si>
+    <t>npoi</t>
+  </si>
+  <si>
+    <t>trfd_m</t>
+  </si>
+  <si>
+    <t>csho</t>
+  </si>
+  <si>
+    <t>Restement magnitude for Nonoperating Income (Expense)</t>
+  </si>
+  <si>
+    <t>Common Shares Outstanding</t>
+  </si>
+  <si>
+    <t>Sale of Common and Preferred Stock</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nonoperating Income (Expense)</t>
+  </si>
+  <si>
+    <t>Importance Value</t>
   </si>
 </sst>
 </file>
@@ -843,7 +873,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -857,7 +887,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -879,6 +908,12 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -904,12 +939,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6177,14 +6214,14 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="13">
         <v>0.83132530000000004</v>
       </c>
       <c r="C2" s="1">
@@ -7029,8 +7066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D96FAC2-DC0D-4E40-A0E9-84734552950F}">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C1:F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7038,541 +7075,712 @@
     <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="56.44140625" customWidth="1"/>
     <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.21875" customWidth="1"/>
+    <col min="5" max="5" width="53.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C1" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="7" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C1" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C2" s="5">
-        <f>C23+1</f>
+      <c r="F1" s="10" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C2" s="14">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="34" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C3" s="5">
-        <f t="shared" ref="C3:C21" si="0">C2+1</f>
+      <c r="F2" s="36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C3" s="14">
+        <f t="shared" ref="C3:C26" si="0">C2+1</f>
         <v>2</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="14" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F3" s="36">
+        <v>79.419404044566207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="5">
+      <c r="C4" s="14">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="14" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C5" s="5">
+      <c r="F4" s="36">
+        <v>75.6368392890179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C5" s="14">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="34" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C6" s="5">
+      <c r="F5" s="36">
+        <v>54.023193069382501</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C6" s="14">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D6" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>138</v>
+      <c r="D6" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6" s="36">
+        <v>51.347698658887602</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C7" s="5">
+      <c r="C7" s="14">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="14" t="s">
         <v>85</v>
+      </c>
+      <c r="F7" s="36">
+        <v>50.552160313428402</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C8" s="5">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C8" s="14">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="34" t="s">
         <v>83</v>
       </c>
+      <c r="F8" s="36">
+        <v>48.270251035754697</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C9" s="5">
+      <c r="C9" s="14">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="34" t="s">
         <v>82</v>
+      </c>
+      <c r="F9" s="36">
+        <v>46.503194830885597</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C10" s="5">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C10" s="14">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C11" s="5">
+      <c r="D10" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="F10" s="36">
+        <v>45.425925946469199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C11" s="14">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="34" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C12" s="5">
+      <c r="F11" s="36">
+        <v>43.1477802278811</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C12" s="14">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="34" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C13" s="5">
+      <c r="F12" s="36">
+        <v>39.966131182752399</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C13" s="14">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="34" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F13" s="36">
+        <v>39.917185640705199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
-      <c r="C14" s="5">
+      <c r="C14" s="14">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="14" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C15" s="5">
+      <c r="F14" s="36">
+        <v>35.975118062265501</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C15" s="14">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="34" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C16" s="5">
+      <c r="F15" s="36">
+        <v>35.231189095811899</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C16" s="14">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="34" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C17" s="5">
+      <c r="F16" s="36">
+        <v>33.539740688030001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="14">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="34" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C18" s="5">
+      <c r="F17" s="36">
+        <v>33.099310039695702</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="14">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="34" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C19" s="5">
+      <c r="F18" s="36">
+        <v>31.1518850864536</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="14">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="34" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C20" s="5">
+      <c r="F19" s="36">
+        <v>30.910892430815998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C20" s="14">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="34" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C21" s="5">
+      <c r="F20" s="36">
+        <v>29.365603588550499</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C21" s="14">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="D21" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>139</v>
+      <c r="D21" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="F21" s="36">
+        <v>28.3540475307537</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C22" s="14">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="E22" s="34" t="s">
+        <v>198</v>
+      </c>
+      <c r="F22" s="36">
+        <v>26.275918825074001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C23" s="14">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>193</v>
+      </c>
+      <c r="E23" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="F23" s="36">
+        <v>24.4141119578148</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="8" t="s">
-        <v>91</v>
+      <c r="C24" s="14">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" s="36">
+        <v>20.941424368782101</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="C25" s="14">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>194</v>
+      </c>
+      <c r="E25" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="F25" s="36">
+        <v>20.836522072360001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
+      <c r="B26" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="C26" s="14">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="E26" s="34" t="s">
+        <v>201</v>
+      </c>
+      <c r="F26" s="36">
+        <v>20.237719735476801</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D26" s="5">
-        <f>C5+1</f>
-        <v>5</v>
-      </c>
-      <c r="E26" s="6" t="s">
+      <c r="B27" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="14">
+        <f>C26+1</f>
+        <v>26</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="E27" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="F27" s="36">
+        <v>20.035942892504998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" s="14">
+        <f>C27+1</f>
+        <v>27</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="F28" s="36">
+        <v>19.631536992822301</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" s="14">
+        <f>C28+1</f>
+        <v>28</v>
+      </c>
+      <c r="D29" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="E29" s="34" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B29" s="9" t="s">
+      <c r="F29" s="36">
+        <v>19.611764948525401</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" s="14">
+        <f>C29+1</f>
+        <v>29</v>
+      </c>
+      <c r="D30" s="34" t="s">
+        <v>196</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="F30" s="36">
+        <v>19.411122985139201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30" s="5">
-        <f>C7+1</f>
-        <v>7</v>
-      </c>
-      <c r="E30" s="5" t="s">
+      <c r="B31" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" s="14">
+        <f>C30+1</f>
+        <v>30</v>
+      </c>
+      <c r="D31" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="E31" s="34" t="s">
+        <v>199</v>
+      </c>
+      <c r="F31" s="36">
+        <v>17.303323591554701</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="14"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="F30" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="D32" s="5">
-        <f>C9+1</f>
-        <v>9</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="10"/>
-      <c r="B41" s="10"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B54" s="12" t="s">
+      <c r="B55" s="11" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B55" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="12"/>
-      <c r="B56" s="12"/>
+      <c r="A56" s="11"/>
+      <c r="B56" s="11"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="12"/>
-      <c r="B57" s="12"/>
+      <c r="A57" s="11"/>
+      <c r="B57" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7609,35 +7817,35 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="26"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="28"/>
+    </row>
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="25"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="D6" s="27"/>
-    </row>
-    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="B7" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>142</v>
-      </c>
       <c r="C7" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>141</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -7655,19 +7863,19 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="17">
+      <c r="A9" s="16">
         <f>A8/SUM(A8:B8)</f>
         <v>0.13654618473895583</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="16">
         <f>B8/SUM(A8:B8)</f>
         <v>0.86345381526104414</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="16">
         <f>C8/SUM(C8:D8)</f>
         <v>0.36546184738955823</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="16">
         <f>D8/SUM(C8:D8)</f>
         <v>0.63453815261044177</v>
       </c>
@@ -7702,338 +7910,338 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
-      <c r="B1" s="30" t="s">
+      <c r="A1" s="11"/>
+      <c r="B1" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="31"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" s="11">
+        <v>53</v>
+      </c>
+      <c r="C3" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="11">
+        <v>19</v>
+      </c>
+      <c r="C4" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="30"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="B3" s="12">
-        <v>53</v>
-      </c>
-      <c r="C3" s="12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="B4" s="12">
-        <v>19</v>
-      </c>
-      <c r="C4" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="B5" s="29">
+      <c r="B5" s="30">
         <f>SUM(B3,C4)/SUM(B3:C4)</f>
         <v>0.6987951807228916</v>
       </c>
-      <c r="C5" s="29"/>
+      <c r="C5" s="30"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="30" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="31"/>
+      <c r="F8" s="12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" s="11">
+        <v>64</v>
+      </c>
+      <c r="C10" s="11">
+        <v>7</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" s="11">
+        <v>8</v>
+      </c>
+      <c r="C11" s="11">
+        <v>4</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="F8" s="13" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="B10" s="12">
-        <v>64</v>
-      </c>
-      <c r="C10" s="12">
-        <v>7</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="B11" s="12">
-        <v>8</v>
-      </c>
-      <c r="C11" s="12">
-        <v>4</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="B12" s="29">
+      <c r="B12" s="30">
         <f>SUM(B10,C11)/SUM(B10:C11)</f>
         <v>0.81927710843373491</v>
       </c>
-      <c r="C12" s="29"/>
-      <c r="F12" s="13" t="s">
+      <c r="C12" s="30"/>
+      <c r="F12" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F13" s="20" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F13" s="21" t="s">
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F14" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F14" s="21" t="s">
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F15" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F15" s="21" t="s">
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F16" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F16" s="13" t="s">
+    </row>
+    <row r="17" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F17" s="12" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="17" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F17" s="13" t="s">
+    <row r="18" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F18" s="20" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="18" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F18" s="21" t="s">
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+    </row>
+    <row r="19" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F19" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-    </row>
-    <row r="19" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F19" s="21" t="s">
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+    </row>
+    <row r="20" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F20" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-    </row>
-    <row r="20" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F20" s="13" t="s">
+    </row>
+    <row r="21" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F21" s="20" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="21" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F21" s="21" t="s">
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+    </row>
+    <row r="22" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F22" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-    </row>
-    <row r="22" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F22" s="13" t="s">
+    </row>
+    <row r="23" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F23" s="12" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="23" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F23" s="13" t="s">
+    <row r="24" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F24" s="20" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="24" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F24" s="21" t="s">
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+    </row>
+    <row r="25" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F25" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-    </row>
-    <row r="25" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F25" s="13" t="s">
+    </row>
+    <row r="26" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F26" s="20" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="26" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F26" s="21" t="s">
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="21"/>
+    </row>
+    <row r="27" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F27" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-    </row>
-    <row r="27" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F27" s="21" t="s">
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+    </row>
+    <row r="28" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F28" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-    </row>
-    <row r="28" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F28" s="21" t="s">
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="21"/>
+    </row>
+    <row r="29" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F29" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-    </row>
-    <row r="29" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F29" s="13" t="s">
+    </row>
+    <row r="30" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F30" s="20" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="30" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F30" s="21" t="s">
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+    </row>
+    <row r="31" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F31" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="22"/>
-      <c r="L30" s="22"/>
-      <c r="M30" s="22"/>
-    </row>
-    <row r="31" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F31" s="13" t="s">
+    </row>
+    <row r="32" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="F32" s="12" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="32" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F32" s="13" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N35" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O35" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="12"/>
-      <c r="B36" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="C36" s="30"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="C36" s="31"/>
       <c r="N36" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="O36" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="O36" s="6" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="37" spans="1:15" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="B37" s="18" t="s">
+      <c r="A37" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C37" s="17" t="s">
         <v>141</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>142</v>
       </c>
       <c r="N37" s="6" t="s">
         <v>54</v>
@@ -8043,30 +8251,30 @@
       </c>
     </row>
     <row r="38" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B38" s="11">
+        <v>64</v>
+      </c>
+      <c r="C38" s="11">
+        <v>6</v>
+      </c>
+      <c r="N38" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="O38" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="B38" s="12">
-        <v>64</v>
-      </c>
-      <c r="C38" s="12">
-        <v>6</v>
-      </c>
-      <c r="N38" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="O38" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="B39" s="12">
+      <c r="B39" s="11">
         <v>8</v>
       </c>
-      <c r="C39" s="12">
+      <c r="C39" s="11">
         <v>5</v>
       </c>
       <c r="N39" s="5" t="s">
@@ -8077,14 +8285,14 @@
       </c>
     </row>
     <row r="40" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="B40" s="29">
+      <c r="A40" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="B40" s="30">
         <f>SUM(B38,C39)/SUM(B38:C39)</f>
         <v>0.83132530120481929</v>
       </c>
-      <c r="C40" s="29"/>
+      <c r="C40" s="30"/>
       <c r="N40" s="5" t="s">
         <v>66</v>
       </c>
@@ -8097,23 +8305,23 @@
         <v>67</v>
       </c>
       <c r="O41" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="N42" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="O42" s="5" t="s">
         <v>177</v>
-      </c>
-      <c r="O42" s="5" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="N43" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O43" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
@@ -8153,225 +8361,225 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
-      <c r="B1" s="30" t="s">
+      <c r="A1" s="11"/>
+      <c r="B1" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="31"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" s="11">
+        <v>67</v>
+      </c>
+      <c r="C3" s="11">
+        <v>7</v>
+      </c>
+      <c r="H3" s="22">
+        <v>1</v>
+      </c>
+      <c r="I3" s="22">
+        <v>85.542169999999999</v>
+      </c>
+      <c r="J3" s="22">
+        <v>88.636359999999996</v>
+      </c>
+      <c r="K3" s="22" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="11">
+        <v>5</v>
+      </c>
+      <c r="C4" s="11">
+        <v>4</v>
+      </c>
+      <c r="H4" s="22">
+        <v>2</v>
+      </c>
+      <c r="I4" s="22">
+        <v>84.337350000000001</v>
+      </c>
+      <c r="J4" s="22">
+        <v>86.426770000000005</v>
+      </c>
+      <c r="K4" s="22" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="30"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="H2" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="I2" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="J2" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="K2" s="33" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="B3" s="12">
-        <v>67</v>
-      </c>
-      <c r="C3" s="12">
-        <v>7</v>
-      </c>
-      <c r="H3" s="32">
-        <v>1</v>
-      </c>
-      <c r="I3" s="32">
-        <v>85.542169999999999</v>
-      </c>
-      <c r="J3" s="32">
-        <v>88.636359999999996</v>
-      </c>
-      <c r="K3" s="32" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="B4" s="12">
-        <v>5</v>
-      </c>
-      <c r="C4" s="12">
-        <v>4</v>
-      </c>
-      <c r="H4" s="32">
-        <v>2</v>
-      </c>
-      <c r="I4" s="32">
-        <v>84.337350000000001</v>
-      </c>
-      <c r="J4" s="32">
-        <v>86.426770000000005</v>
-      </c>
-      <c r="K4" s="32" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="B5" s="29">
+      <c r="B5" s="30">
         <f>SUM(B3,C4)/SUM(B3:C4)</f>
         <v>0.85542168674698793</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="H5" s="32">
+      <c r="C5" s="30"/>
+      <c r="H5" s="22">
         <v>3</v>
       </c>
-      <c r="I5" s="32">
+      <c r="I5" s="22">
         <v>84.337350000000001</v>
       </c>
-      <c r="J5" s="32">
+      <c r="J5" s="22">
         <v>85.984849999999994</v>
       </c>
-      <c r="K5" s="32" t="s">
+      <c r="K5" s="22" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H6" s="22">
+        <v>4</v>
+      </c>
+      <c r="I6" s="22">
+        <v>84.337350000000001</v>
+      </c>
+      <c r="J6" s="22">
+        <v>79.545450000000002</v>
+      </c>
+      <c r="K6" s="22" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="H6" s="32">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" s="31"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" s="11">
+        <v>66</v>
+      </c>
+      <c r="C12" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" s="11">
+        <v>6</v>
+      </c>
+      <c r="C13" s="11">
         <v>4</v>
       </c>
-      <c r="I6" s="32">
-        <v>84.337350000000001</v>
-      </c>
-      <c r="J6" s="32">
-        <v>79.545450000000002</v>
-      </c>
-      <c r="K6" s="32" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="30" t="s">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="C10" s="30"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="B12" s="12">
-        <v>66</v>
-      </c>
-      <c r="C12" s="12">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="B13" s="12">
-        <v>6</v>
-      </c>
-      <c r="C13" s="12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="B14" s="29">
+      <c r="B14" s="30">
         <f>SUM(B12,C13)/SUM(B12:C13)</f>
         <v>0.84337349397590367</v>
       </c>
-      <c r="C14" s="29"/>
+      <c r="C14" s="30"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="30" t="s">
+      <c r="A19" s="11"/>
+      <c r="B19" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" s="31"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B21" s="11">
+        <v>66</v>
+      </c>
+      <c r="C21" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22" s="11">
+        <v>6</v>
+      </c>
+      <c r="C22" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="C19" s="30"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="B21" s="12">
-        <v>66</v>
-      </c>
-      <c r="C21" s="12">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="B22" s="12">
-        <v>6</v>
-      </c>
-      <c r="C22" s="12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="B23" s="29">
+      <c r="B23" s="30">
         <f>SUM(B21,C22)/SUM(B21:C22)</f>
         <v>0.84337349397590367</v>
       </c>
-      <c r="C23" s="29"/>
+      <c r="C23" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B23:C23"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B23:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8381,7 +8589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC64DDE-0857-4BC0-9FEC-5901E9ECC32B}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P36" sqref="P36"/>
     </sheetView>
   </sheetViews>
@@ -8393,15 +8601,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" s="1">
         <v>0.85542169999999995</v>
@@ -8409,7 +8617,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B3" s="1">
         <v>0.83130000000000004</v>
@@ -8417,7 +8625,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B4" s="1">
         <v>0.74698799999999999</v>
@@ -8425,7 +8633,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B5" s="1">
         <v>0.77108429999999994</v>
@@ -8433,7 +8641,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B6" s="1">
         <v>0.69879519999999995</v>
@@ -8441,15 +8649,15 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B23" s="1">
         <v>0.88636360000000003</v>
@@ -8457,7 +8665,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B24" s="1">
         <v>0.75378789999999996</v>
@@ -8465,7 +8673,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B25" s="1">
         <v>0.79545449999999995</v>
@@ -8473,7 +8681,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B26" s="1">
         <v>0.62752529999999995</v>
@@ -8481,7 +8689,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B27" s="1">
         <v>0.53093429999999997</v>

</xml_diff>